<commit_message>
Product management code updated
</commit_message>
<xml_diff>
--- a/frontend/public/Multiturn Actuators.xlsx
+++ b/frontend/public/Multiturn Actuators.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/20a867eda9f4d836/Documents/Auma_Doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Documents\Auma_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4CF4AFFF-08FD-4A99-857C-3130CFEA3C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{629227E6-E5A0-4B0E-B822-81A4A2D53976}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9246E70-2370-444A-9FCA-F00EA694194B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>